<commit_message>
Correct valuset references #10 #34
</commit_message>
<xml_diff>
--- a/docs/CareConnect-HeartRate-Observation-1.xlsx
+++ b/docs/CareConnect-HeartRate-Observation-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6627" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6627" uniqueCount="661">
   <si>
     <t>Path</t>
   </si>
@@ -915,9 +915,6 @@
   </si>
   <si>
     <t>loinc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This value set indicates the allowed vital sign result types. </t>
   </si>
   <si>
     <t>Observation.code.coding.id</t>
@@ -6672,7 +6669,7 @@
         <v>79</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="Y38" t="s" s="2">
         <v>279</v>
@@ -6728,7 +6725,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6843,7 +6840,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6960,7 +6957,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -7002,7 +6999,7 @@
       </c>
       <c r="P41" s="2"/>
       <c r="Q41" t="s" s="2">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="R41" t="s" s="2">
         <v>45</v>
@@ -7079,7 +7076,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -7196,7 +7193,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -7236,7 +7233,7 @@
       </c>
       <c r="P43" s="2"/>
       <c r="Q43" t="s" s="2">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="R43" t="s" s="2">
         <v>45</v>
@@ -7313,7 +7310,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -7430,7 +7427,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -7552,7 +7549,7 @@
         <v>288</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C46" t="s" s="2">
         <v>45</v>
@@ -7670,7 +7667,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -7785,7 +7782,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7811,10 +7808,10 @@
         <v>102</v>
       </c>
       <c r="K48" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="L48" t="s" s="2">
         <v>302</v>
-      </c>
-      <c r="L48" t="s" s="2">
-        <v>303</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -7900,10 +7897,10 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C49" t="s" s="2">
         <v>45</v>
@@ -7925,13 +7922,13 @@
         <v>45</v>
       </c>
       <c r="J49" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="K49" t="s" s="2">
         <v>305</v>
       </c>
-      <c r="K49" t="s" s="2">
+      <c r="L49" t="s" s="2">
         <v>306</v>
-      </c>
-      <c r="L49" t="s" s="2">
-        <v>307</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -8017,7 +8014,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -8059,7 +8056,7 @@
       </c>
       <c r="P50" s="2"/>
       <c r="Q50" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="R50" t="s" s="2">
         <v>45</v>
@@ -8136,7 +8133,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -8253,7 +8250,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -8293,7 +8290,7 @@
       </c>
       <c r="P52" s="2"/>
       <c r="Q52" t="s" s="2">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="R52" t="s" s="2">
         <v>45</v>
@@ -8370,7 +8367,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -8410,7 +8407,7 @@
       </c>
       <c r="P53" s="2"/>
       <c r="Q53" t="s" s="2">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R53" t="s" s="2">
         <v>45</v>
@@ -8487,7 +8484,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -8606,7 +8603,7 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -8725,7 +8722,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -8748,19 +8745,19 @@
         <v>57</v>
       </c>
       <c r="J56" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="K56" t="s" s="2">
         <v>313</v>
       </c>
-      <c r="K56" t="s" s="2">
+      <c r="L56" t="s" s="2">
         <v>314</v>
       </c>
-      <c r="L56" t="s" s="2">
+      <c r="M56" t="s" s="2">
         <v>315</v>
       </c>
-      <c r="M56" t="s" s="2">
+      <c r="N56" t="s" s="2">
         <v>316</v>
-      </c>
-      <c r="N56" t="s" s="2">
-        <v>317</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>45</v>
@@ -8809,7 +8806,7 @@
         <v>45</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>43</v>
@@ -8824,19 +8821,19 @@
         <v>45</v>
       </c>
       <c r="AJ56" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="AK56" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL56" t="s" s="2">
         <v>318</v>
       </c>
-      <c r="AK56" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL56" t="s" s="2">
+      <c r="AM56" t="s" s="2">
         <v>319</v>
       </c>
-      <c r="AM56" t="s" s="2">
+      <c r="AN56" t="s" s="2">
         <v>320</v>
-      </c>
-      <c r="AN56" t="s" s="2">
-        <v>321</v>
       </c>
       <c r="AO56" t="s" s="2">
         <v>45</v>
@@ -8844,11 +8841,11 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
@@ -8867,19 +8864,19 @@
         <v>45</v>
       </c>
       <c r="J57" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="K57" t="s" s="2">
         <v>324</v>
       </c>
-      <c r="K57" t="s" s="2">
+      <c r="L57" t="s" s="2">
         <v>325</v>
       </c>
-      <c r="L57" t="s" s="2">
+      <c r="M57" t="s" s="2">
         <v>326</v>
       </c>
-      <c r="M57" t="s" s="2">
+      <c r="N57" t="s" s="2">
         <v>327</v>
-      </c>
-      <c r="N57" t="s" s="2">
-        <v>328</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>45</v>
@@ -8928,7 +8925,7 @@
         <v>45</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>43</v>
@@ -8943,19 +8940,19 @@
         <v>45</v>
       </c>
       <c r="AJ57" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="AK57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL57" t="s" s="2">
         <v>329</v>
       </c>
-      <c r="AK57" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL57" t="s" s="2">
+      <c r="AM57" t="s" s="2">
         <v>330</v>
       </c>
-      <c r="AM57" t="s" s="2">
+      <c r="AN57" t="s" s="2">
         <v>331</v>
-      </c>
-      <c r="AN57" t="s" s="2">
-        <v>332</v>
       </c>
       <c r="AO57" t="s" s="2">
         <v>45</v>
@@ -8963,11 +8960,11 @@
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" t="s" s="2">
@@ -8986,19 +8983,19 @@
         <v>57</v>
       </c>
       <c r="J58" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="K58" t="s" s="2">
         <v>335</v>
       </c>
-      <c r="K58" t="s" s="2">
+      <c r="L58" t="s" s="2">
         <v>336</v>
       </c>
-      <c r="L58" t="s" s="2">
+      <c r="M58" t="s" s="2">
         <v>337</v>
       </c>
-      <c r="M58" t="s" s="2">
+      <c r="N58" t="s" s="2">
         <v>338</v>
-      </c>
-      <c r="N58" t="s" s="2">
-        <v>339</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>45</v>
@@ -9047,7 +9044,7 @@
         <v>45</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>43</v>
@@ -9062,19 +9059,19 @@
         <v>45</v>
       </c>
       <c r="AJ58" t="s" s="2">
+        <v>339</v>
+      </c>
+      <c r="AK58" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL58" t="s" s="2">
         <v>340</v>
       </c>
-      <c r="AK58" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL58" t="s" s="2">
+      <c r="AM58" t="s" s="2">
         <v>341</v>
       </c>
-      <c r="AM58" t="s" s="2">
+      <c r="AN58" t="s" s="2">
         <v>342</v>
-      </c>
-      <c r="AN58" t="s" s="2">
-        <v>343</v>
       </c>
       <c r="AO58" t="s" s="2">
         <v>45</v>
@@ -9082,7 +9079,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -9105,16 +9102,16 @@
         <v>57</v>
       </c>
       <c r="J59" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="K59" t="s" s="2">
         <v>345</v>
       </c>
-      <c r="K59" t="s" s="2">
+      <c r="L59" t="s" s="2">
         <v>346</v>
       </c>
-      <c r="L59" t="s" s="2">
+      <c r="M59" t="s" s="2">
         <v>347</v>
-      </c>
-      <c r="M59" t="s" s="2">
-        <v>348</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" t="s" s="2">
@@ -9164,7 +9161,7 @@
         <v>45</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>43</v>
@@ -9185,13 +9182,13 @@
         <v>45</v>
       </c>
       <c r="AL59" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="AM59" t="s" s="2">
         <v>349</v>
       </c>
-      <c r="AM59" t="s" s="2">
+      <c r="AN59" t="s" s="2">
         <v>350</v>
-      </c>
-      <c r="AN59" t="s" s="2">
-        <v>351</v>
       </c>
       <c r="AO59" t="s" s="2">
         <v>45</v>
@@ -9199,7 +9196,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -9222,17 +9219,17 @@
         <v>57</v>
       </c>
       <c r="J60" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="K60" t="s" s="2">
         <v>353</v>
       </c>
-      <c r="K60" t="s" s="2">
+      <c r="L60" t="s" s="2">
         <v>354</v>
-      </c>
-      <c r="L60" t="s" s="2">
-        <v>355</v>
       </c>
       <c r="M60" s="2"/>
       <c r="N60" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>45</v>
@@ -9281,7 +9278,7 @@
         <v>45</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>43</v>
@@ -9296,19 +9293,19 @@
         <v>45</v>
       </c>
       <c r="AJ60" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="AK60" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL60" t="s" s="2">
         <v>357</v>
       </c>
-      <c r="AK60" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL60" t="s" s="2">
+      <c r="AM60" t="s" s="2">
         <v>358</v>
       </c>
-      <c r="AM60" t="s" s="2">
+      <c r="AN60" t="s" s="2">
         <v>359</v>
-      </c>
-      <c r="AN60" t="s" s="2">
-        <v>360</v>
       </c>
       <c r="AO60" t="s" s="2">
         <v>45</v>
@@ -9316,7 +9313,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -9339,19 +9336,19 @@
         <v>57</v>
       </c>
       <c r="J61" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="K61" t="s" s="2">
         <v>362</v>
       </c>
-      <c r="K61" t="s" s="2">
+      <c r="L61" t="s" s="2">
         <v>363</v>
       </c>
-      <c r="L61" t="s" s="2">
+      <c r="M61" t="s" s="2">
         <v>364</v>
       </c>
-      <c r="M61" t="s" s="2">
+      <c r="N61" t="s" s="2">
         <v>365</v>
-      </c>
-      <c r="N61" t="s" s="2">
-        <v>366</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>45</v>
@@ -9388,55 +9385,55 @@
         <v>45</v>
       </c>
       <c r="AA61" t="s" s="2">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AB61" s="2"/>
       <c r="AC61" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD61" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="AE61" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="AF61" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG61" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH61" t="s" s="2">
         <v>368</v>
       </c>
-      <c r="AE61" t="s" s="2">
-        <v>361</v>
-      </c>
-      <c r="AF61" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG61" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH61" t="s" s="2">
+      <c r="AI61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ61" t="s" s="2">
         <v>369</v>
       </c>
-      <c r="AI61" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ61" t="s" s="2">
+      <c r="AK61" t="s" s="2">
         <v>370</v>
       </c>
-      <c r="AK61" t="s" s="2">
+      <c r="AL61" t="s" s="2">
         <v>371</v>
       </c>
-      <c r="AL61" t="s" s="2">
+      <c r="AM61" t="s" s="2">
         <v>372</v>
       </c>
-      <c r="AM61" t="s" s="2">
+      <c r="AN61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO61" t="s" s="2">
         <v>373</v>
-      </c>
-      <c r="AN61" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO61" t="s" s="2">
-        <v>374</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C62" t="s" s="2">
         <v>45</v>
@@ -9458,19 +9455,19 @@
         <v>57</v>
       </c>
       <c r="J62" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="K62" t="s" s="2">
         <v>362</v>
       </c>
-      <c r="K62" t="s" s="2">
+      <c r="L62" t="s" s="2">
         <v>363</v>
       </c>
-      <c r="L62" t="s" s="2">
+      <c r="M62" t="s" s="2">
         <v>364</v>
       </c>
-      <c r="M62" t="s" s="2">
+      <c r="N62" t="s" s="2">
         <v>365</v>
-      </c>
-      <c r="N62" t="s" s="2">
-        <v>366</v>
       </c>
       <c r="O62" t="s" s="2">
         <v>45</v>
@@ -9498,11 +9495,11 @@
         <v>136</v>
       </c>
       <c r="X62" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="Y62" t="s" s="2">
         <v>376</v>
       </c>
-      <c r="Y62" t="s" s="2">
-        <v>377</v>
-      </c>
       <c r="Z62" t="s" s="2">
         <v>45</v>
       </c>
@@ -9519,7 +9516,7 @@
         <v>45</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>43</v>
@@ -9528,33 +9525,33 @@
         <v>56</v>
       </c>
       <c r="AH62" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="AI62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ62" t="s" s="2">
         <v>369</v>
       </c>
-      <c r="AI62" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ62" t="s" s="2">
+      <c r="AK62" t="s" s="2">
         <v>370</v>
       </c>
-      <c r="AK62" t="s" s="2">
+      <c r="AL62" t="s" s="2">
         <v>371</v>
       </c>
-      <c r="AL62" t="s" s="2">
+      <c r="AM62" t="s" s="2">
         <v>372</v>
       </c>
-      <c r="AM62" t="s" s="2">
+      <c r="AN62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO62" t="s" s="2">
         <v>373</v>
-      </c>
-      <c r="AN62" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO62" t="s" s="2">
-        <v>374</v>
       </c>
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -9669,7 +9666,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -9786,7 +9783,7 @@
     </row>
     <row r="65">
       <c r="A65" t="s" s="2">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -9809,19 +9806,19 @@
         <v>57</v>
       </c>
       <c r="J65" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="K65" t="s" s="2">
         <v>381</v>
       </c>
-      <c r="K65" t="s" s="2">
+      <c r="L65" t="s" s="2">
         <v>382</v>
       </c>
-      <c r="L65" t="s" s="2">
+      <c r="M65" t="s" s="2">
         <v>383</v>
       </c>
-      <c r="M65" t="s" s="2">
+      <c r="N65" t="s" s="2">
         <v>384</v>
-      </c>
-      <c r="N65" t="s" s="2">
-        <v>385</v>
       </c>
       <c r="O65" t="s" s="2">
         <v>45</v>
@@ -9870,31 +9867,31 @@
         <v>45</v>
       </c>
       <c r="AE65" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="AF65" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG65" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL65" t="s" s="2">
         <v>386</v>
       </c>
-      <c r="AF65" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG65" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH65" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI65" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ65" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK65" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL65" t="s" s="2">
+      <c r="AM65" t="s" s="2">
         <v>387</v>
-      </c>
-      <c r="AM65" t="s" s="2">
-        <v>388</v>
       </c>
       <c r="AN65" t="s" s="2">
         <v>45</v>
@@ -9905,7 +9902,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -9931,22 +9928,22 @@
         <v>75</v>
       </c>
       <c r="K66" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="L66" t="s" s="2">
         <v>390</v>
       </c>
-      <c r="L66" t="s" s="2">
+      <c r="M66" t="s" s="2">
         <v>391</v>
       </c>
-      <c r="M66" t="s" s="2">
+      <c r="N66" t="s" s="2">
         <v>392</v>
       </c>
-      <c r="N66" t="s" s="2">
+      <c r="O66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P66" t="s" s="2">
         <v>393</v>
-      </c>
-      <c r="O66" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="P66" t="s" s="2">
-        <v>394</v>
       </c>
       <c r="Q66" t="s" s="2">
         <v>45</v>
@@ -9970,52 +9967,52 @@
         <v>136</v>
       </c>
       <c r="X66" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="Y66" t="s" s="2">
         <v>395</v>
       </c>
-      <c r="Y66" t="s" s="2">
+      <c r="Z66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE66" t="s" s="2">
         <v>396</v>
       </c>
-      <c r="Z66" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA66" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB66" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC66" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD66" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE66" t="s" s="2">
+      <c r="AF66" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG66" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL66" t="s" s="2">
         <v>397</v>
       </c>
-      <c r="AF66" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG66" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH66" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI66" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ66" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK66" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL66" t="s" s="2">
+      <c r="AM66" t="s" s="2">
         <v>398</v>
-      </c>
-      <c r="AM66" t="s" s="2">
-        <v>399</v>
       </c>
       <c r="AN66" t="s" s="2">
         <v>45</v>
@@ -10026,7 +10023,7 @@
     </row>
     <row r="67">
       <c r="A67" t="s" s="2">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -10052,14 +10049,14 @@
         <v>120</v>
       </c>
       <c r="K67" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="L67" t="s" s="2">
         <v>401</v>
-      </c>
-      <c r="L67" t="s" s="2">
-        <v>402</v>
       </c>
       <c r="M67" s="2"/>
       <c r="N67" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="O67" t="s" s="2">
         <v>45</v>
@@ -10108,31 +10105,31 @@
         <v>45</v>
       </c>
       <c r="AE67" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="AF67" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG67" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL67" t="s" s="2">
         <v>404</v>
       </c>
-      <c r="AF67" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG67" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL67" t="s" s="2">
+      <c r="AM67" t="s" s="2">
         <v>405</v>
-      </c>
-      <c r="AM67" t="s" s="2">
-        <v>406</v>
       </c>
       <c r="AN67" t="s" s="2">
         <v>45</v>
@@ -10143,7 +10140,7 @@
     </row>
     <row r="68">
       <c r="A68" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -10169,87 +10166,87 @@
         <v>69</v>
       </c>
       <c r="K68" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="L68" t="s" s="2">
         <v>408</v>
-      </c>
-      <c r="L68" t="s" s="2">
-        <v>409</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" t="s" s="2">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="O68" t="s" s="2">
         <v>45</v>
       </c>
       <c r="P68" s="2"/>
       <c r="Q68" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="R68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE68" t="s" s="2">
         <v>411</v>
       </c>
-      <c r="R68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="S68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Y68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Z68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE68" t="s" s="2">
+      <c r="AF68" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG68" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH68" t="s" s="2">
         <v>412</v>
       </c>
-      <c r="AF68" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG68" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH68" t="s" s="2">
+      <c r="AI68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL68" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="AM68" t="s" s="2">
         <v>413</v>
-      </c>
-      <c r="AI68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL68" t="s" s="2">
-        <v>405</v>
-      </c>
-      <c r="AM68" t="s" s="2">
-        <v>414</v>
       </c>
       <c r="AN68" t="s" s="2">
         <v>45</v>
@@ -10260,7 +10257,7 @@
     </row>
     <row r="69">
       <c r="A69" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -10286,89 +10283,89 @@
         <v>75</v>
       </c>
       <c r="K69" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="L69" t="s" s="2">
         <v>416</v>
       </c>
-      <c r="L69" t="s" s="2">
+      <c r="M69" t="s" s="2">
         <v>417</v>
       </c>
-      <c r="M69" t="s" s="2">
+      <c r="N69" t="s" s="2">
         <v>418</v>
-      </c>
-      <c r="N69" t="s" s="2">
-        <v>419</v>
       </c>
       <c r="O69" t="s" s="2">
         <v>45</v>
       </c>
       <c r="P69" s="2"/>
       <c r="Q69" t="s" s="2">
+        <v>419</v>
+      </c>
+      <c r="R69" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S69" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T69" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U69" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V69" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W69" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X69" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y69" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z69" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA69" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB69" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC69" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD69" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE69" t="s" s="2">
         <v>420</v>
       </c>
-      <c r="R69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="S69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Y69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Z69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE69" t="s" s="2">
+      <c r="AF69" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG69" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH69" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI69" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ69" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK69" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL69" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="AM69" t="s" s="2">
         <v>421</v>
-      </c>
-      <c r="AF69" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG69" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL69" t="s" s="2">
-        <v>405</v>
-      </c>
-      <c r="AM69" t="s" s="2">
-        <v>422</v>
       </c>
       <c r="AN69" t="s" s="2">
         <v>45</v>
@@ -10379,7 +10376,7 @@
     </row>
     <row r="70">
       <c r="A70" t="s" s="2">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -10405,16 +10402,16 @@
         <v>142</v>
       </c>
       <c r="K70" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="L70" t="s" s="2">
         <v>424</v>
       </c>
-      <c r="L70" t="s" s="2">
+      <c r="M70" t="s" s="2">
         <v>425</v>
       </c>
-      <c r="M70" t="s" s="2">
+      <c r="N70" t="s" s="2">
         <v>426</v>
-      </c>
-      <c r="N70" t="s" s="2">
-        <v>427</v>
       </c>
       <c r="O70" t="s" s="2">
         <v>45</v>
@@ -10442,43 +10439,43 @@
         <v>79</v>
       </c>
       <c r="X70" t="s" s="2">
+        <v>427</v>
+      </c>
+      <c r="Y70" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z70" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA70" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB70" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC70" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD70" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE70" t="s" s="2">
+        <v>422</v>
+      </c>
+      <c r="AF70" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG70" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH70" t="s" s="2">
         <v>428</v>
       </c>
-      <c r="Y70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Z70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE70" t="s" s="2">
-        <v>423</v>
-      </c>
-      <c r="AF70" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG70" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH70" t="s" s="2">
-        <v>429</v>
-      </c>
       <c r="AI70" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ70" t="s" s="2">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AK70" t="s" s="2">
         <v>45</v>
@@ -10487,7 +10484,7 @@
         <v>99</v>
       </c>
       <c r="AM70" t="s" s="2">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="AN70" t="s" s="2">
         <v>45</v>
@@ -10498,7 +10495,7 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -10613,7 +10610,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -10730,7 +10727,7 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -10849,7 +10846,7 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -10964,7 +10961,7 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
@@ -11081,7 +11078,7 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -11200,7 +11197,7 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -11317,7 +11314,7 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -11434,7 +11431,7 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -11551,7 +11548,7 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -11670,7 +11667,7 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
@@ -11789,11 +11786,11 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" t="s" s="2">
@@ -11815,14 +11812,14 @@
         <v>142</v>
       </c>
       <c r="K82" t="s" s="2">
+        <v>443</v>
+      </c>
+      <c r="L82" t="s" s="2">
         <v>444</v>
-      </c>
-      <c r="L82" t="s" s="2">
-        <v>445</v>
       </c>
       <c r="M82" s="2"/>
       <c r="N82" t="s" s="2">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="O82" t="s" s="2">
         <v>45</v>
@@ -11850,63 +11847,63 @@
         <v>79</v>
       </c>
       <c r="X82" t="s" s="2">
+        <v>446</v>
+      </c>
+      <c r="Y82" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z82" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA82" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB82" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC82" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD82" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE82" t="s" s="2">
+        <v>441</v>
+      </c>
+      <c r="AF82" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG82" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH82" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI82" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ82" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK82" t="s" s="2">
         <v>447</v>
       </c>
-      <c r="Y82" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Z82" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA82" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB82" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC82" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD82" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE82" t="s" s="2">
-        <v>442</v>
-      </c>
-      <c r="AF82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG82" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH82" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI82" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ82" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK82" t="s" s="2">
+      <c r="AL82" t="s" s="2">
         <v>448</v>
       </c>
-      <c r="AL82" t="s" s="2">
+      <c r="AM82" t="s" s="2">
         <v>449</v>
       </c>
-      <c r="AM82" t="s" s="2">
+      <c r="AN82" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO82" t="s" s="2">
         <v>450</v>
-      </c>
-      <c r="AN82" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO82" t="s" s="2">
-        <v>451</v>
       </c>
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
@@ -11932,14 +11929,14 @@
         <v>120</v>
       </c>
       <c r="K83" t="s" s="2">
+        <v>452</v>
+      </c>
+      <c r="L83" t="s" s="2">
         <v>453</v>
-      </c>
-      <c r="L83" t="s" s="2">
-        <v>454</v>
       </c>
       <c r="M83" s="2"/>
       <c r="N83" t="s" s="2">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="O83" t="s" s="2">
         <v>45</v>
@@ -11988,7 +11985,7 @@
         <v>45</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="AF83" t="s" s="2">
         <v>43</v>
@@ -12003,16 +12000,16 @@
         <v>45</v>
       </c>
       <c r="AJ83" t="s" s="2">
+        <v>455</v>
+      </c>
+      <c r="AK83" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL83" t="s" s="2">
         <v>456</v>
       </c>
-      <c r="AK83" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL83" t="s" s="2">
+      <c r="AM83" t="s" s="2">
         <v>457</v>
-      </c>
-      <c r="AM83" t="s" s="2">
-        <v>458</v>
       </c>
       <c r="AN83" t="s" s="2">
         <v>45</v>
@@ -12023,7 +12020,7 @@
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
@@ -12049,13 +12046,13 @@
         <v>142</v>
       </c>
       <c r="K84" t="s" s="2">
+        <v>459</v>
+      </c>
+      <c r="L84" t="s" s="2">
         <v>460</v>
       </c>
-      <c r="L84" t="s" s="2">
+      <c r="M84" t="s" s="2">
         <v>461</v>
-      </c>
-      <c r="M84" t="s" s="2">
-        <v>462</v>
       </c>
       <c r="N84" s="2"/>
       <c r="O84" t="s" s="2">
@@ -12081,66 +12078,66 @@
         <v>45</v>
       </c>
       <c r="W84" t="s" s="2">
+        <v>462</v>
+      </c>
+      <c r="X84" t="s" s="2">
         <v>463</v>
       </c>
-      <c r="X84" t="s" s="2">
+      <c r="Y84" t="s" s="2">
         <v>464</v>
       </c>
-      <c r="Y84" t="s" s="2">
+      <c r="Z84" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA84" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB84" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC84" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD84" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE84" t="s" s="2">
+        <v>458</v>
+      </c>
+      <c r="AF84" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG84" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH84" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI84" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ84" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK84" t="s" s="2">
         <v>465</v>
       </c>
-      <c r="Z84" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA84" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB84" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC84" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD84" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE84" t="s" s="2">
-        <v>459</v>
-      </c>
-      <c r="AF84" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG84" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH84" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI84" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ84" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK84" t="s" s="2">
+      <c r="AL84" t="s" s="2">
         <v>466</v>
       </c>
-      <c r="AL84" t="s" s="2">
+      <c r="AM84" t="s" s="2">
         <v>467</v>
       </c>
-      <c r="AM84" t="s" s="2">
+      <c r="AN84" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO84" t="s" s="2">
         <v>468</v>
-      </c>
-      <c r="AN84" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO84" t="s" s="2">
-        <v>469</v>
       </c>
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" t="s" s="2">
@@ -12255,7 +12252,7 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" t="s" s="2">
@@ -12372,7 +12369,7 @@
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" t="s" s="2">
@@ -12444,7 +12441,7 @@
         <v>45</v>
       </c>
       <c r="AA87" t="s" s="2">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="AB87" s="2"/>
       <c r="AC87" t="s" s="2">
@@ -12489,10 +12486,10 @@
     </row>
     <row r="88" hidden="true">
       <c r="A88" t="s" s="2">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B88" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C88" t="s" s="2">
         <v>45</v>
@@ -12551,13 +12548,13 @@
         <v>45</v>
       </c>
       <c r="W88" t="s" s="2">
+        <v>473</v>
+      </c>
+      <c r="X88" t="s" s="2">
         <v>474</v>
       </c>
-      <c r="X88" t="s" s="2">
+      <c r="Y88" t="s" s="2">
         <v>475</v>
-      </c>
-      <c r="Y88" t="s" s="2">
-        <v>476</v>
       </c>
       <c r="Z88" t="s" s="2">
         <v>45</v>
@@ -12610,7 +12607,7 @@
     </row>
     <row r="89" hidden="true">
       <c r="A89" t="s" s="2">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" t="s" s="2">
@@ -12725,7 +12722,7 @@
     </row>
     <row r="90" hidden="true">
       <c r="A90" t="s" s="2">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" t="s" s="2">
@@ -12751,10 +12748,10 @@
         <v>102</v>
       </c>
       <c r="K90" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="L90" t="s" s="2">
         <v>302</v>
-      </c>
-      <c r="L90" t="s" s="2">
-        <v>303</v>
       </c>
       <c r="M90" s="2"/>
       <c r="N90" s="2"/>
@@ -12840,10 +12837,10 @@
     </row>
     <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B91" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C91" t="s" s="2">
         <v>45</v>
@@ -12865,13 +12862,13 @@
         <v>45</v>
       </c>
       <c r="J91" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="K91" t="s" s="2">
         <v>305</v>
       </c>
-      <c r="K91" t="s" s="2">
+      <c r="L91" t="s" s="2">
         <v>306</v>
-      </c>
-      <c r="L91" t="s" s="2">
-        <v>307</v>
       </c>
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
@@ -12957,7 +12954,7 @@
     </row>
     <row r="92" hidden="true">
       <c r="A92" t="s" s="2">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" t="s" s="2">
@@ -12999,7 +12996,7 @@
       </c>
       <c r="P92" s="2"/>
       <c r="Q92" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="R92" t="s" s="2">
         <v>45</v>
@@ -13076,7 +13073,7 @@
     </row>
     <row r="93" hidden="true">
       <c r="A93" t="s" s="2">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" t="s" s="2">
@@ -13193,7 +13190,7 @@
     </row>
     <row r="94" hidden="true">
       <c r="A94" t="s" s="2">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" t="s" s="2">
@@ -13310,7 +13307,7 @@
     </row>
     <row r="95" hidden="true">
       <c r="A95" t="s" s="2">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" t="s" s="2">
@@ -13427,7 +13424,7 @@
     </row>
     <row r="96" hidden="true">
       <c r="A96" t="s" s="2">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" t="s" s="2">
@@ -13546,7 +13543,7 @@
     </row>
     <row r="97" hidden="true">
       <c r="A97" t="s" s="2">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" t="s" s="2">
@@ -13665,7 +13662,7 @@
     </row>
     <row r="98" hidden="true">
       <c r="A98" t="s" s="2">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" t="s" s="2">
@@ -13691,16 +13688,16 @@
         <v>142</v>
       </c>
       <c r="K98" t="s" s="2">
+        <v>485</v>
+      </c>
+      <c r="L98" t="s" s="2">
         <v>486</v>
       </c>
-      <c r="L98" t="s" s="2">
+      <c r="M98" t="s" s="2">
         <v>487</v>
       </c>
-      <c r="M98" t="s" s="2">
+      <c r="N98" t="s" s="2">
         <v>488</v>
-      </c>
-      <c r="N98" t="s" s="2">
-        <v>489</v>
       </c>
       <c r="O98" t="s" s="2">
         <v>45</v>
@@ -13725,55 +13722,55 @@
         <v>45</v>
       </c>
       <c r="W98" t="s" s="2">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="X98" t="s" s="2">
+        <v>489</v>
+      </c>
+      <c r="Y98" t="s" s="2">
         <v>490</v>
       </c>
-      <c r="Y98" t="s" s="2">
+      <c r="Z98" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA98" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB98" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC98" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD98" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE98" t="s" s="2">
+        <v>484</v>
+      </c>
+      <c r="AF98" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG98" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH98" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI98" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ98" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK98" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL98" t="s" s="2">
         <v>491</v>
       </c>
-      <c r="Z98" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA98" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB98" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC98" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD98" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE98" t="s" s="2">
-        <v>485</v>
-      </c>
-      <c r="AF98" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG98" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH98" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI98" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ98" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK98" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL98" t="s" s="2">
+      <c r="AM98" t="s" s="2">
         <v>492</v>
-      </c>
-      <c r="AM98" t="s" s="2">
-        <v>493</v>
       </c>
       <c r="AN98" t="s" s="2">
         <v>45</v>
@@ -13784,7 +13781,7 @@
     </row>
     <row r="99" hidden="true">
       <c r="A99" t="s" s="2">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B99" s="2"/>
       <c r="C99" t="s" s="2">
@@ -13899,7 +13896,7 @@
     </row>
     <row r="100" hidden="true">
       <c r="A100" t="s" s="2">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" t="s" s="2">
@@ -14016,7 +14013,7 @@
     </row>
     <row r="101" hidden="true">
       <c r="A101" t="s" s="2">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" t="s" s="2">
@@ -14088,7 +14085,7 @@
         <v>45</v>
       </c>
       <c r="AA101" t="s" s="2">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="AB101" s="2"/>
       <c r="AC101" t="s" s="2">
@@ -14133,10 +14130,10 @@
     </row>
     <row r="102" hidden="true">
       <c r="A102" t="s" s="2">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B102" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C102" t="s" s="2">
         <v>45</v>
@@ -14195,13 +14192,13 @@
         <v>45</v>
       </c>
       <c r="W102" t="s" s="2">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="X102" t="s" s="2">
+        <v>496</v>
+      </c>
+      <c r="Y102" t="s" s="2">
         <v>497</v>
-      </c>
-      <c r="Y102" t="s" s="2">
-        <v>498</v>
       </c>
       <c r="Z102" t="s" s="2">
         <v>45</v>
@@ -14254,7 +14251,7 @@
     </row>
     <row r="103" hidden="true">
       <c r="A103" t="s" s="2">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B103" s="2"/>
       <c r="C103" t="s" s="2">
@@ -14369,7 +14366,7 @@
     </row>
     <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B104" s="2"/>
       <c r="C104" t="s" s="2">
@@ -14395,10 +14392,10 @@
         <v>102</v>
       </c>
       <c r="K104" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="L104" t="s" s="2">
         <v>302</v>
-      </c>
-      <c r="L104" t="s" s="2">
-        <v>303</v>
       </c>
       <c r="M104" s="2"/>
       <c r="N104" s="2"/>
@@ -14484,10 +14481,10 @@
     </row>
     <row r="105" hidden="true">
       <c r="A105" t="s" s="2">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B105" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C105" t="s" s="2">
         <v>45</v>
@@ -14509,13 +14506,13 @@
         <v>45</v>
       </c>
       <c r="J105" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="K105" t="s" s="2">
         <v>305</v>
       </c>
-      <c r="K105" t="s" s="2">
+      <c r="L105" t="s" s="2">
         <v>306</v>
-      </c>
-      <c r="L105" t="s" s="2">
-        <v>307</v>
       </c>
       <c r="M105" s="2"/>
       <c r="N105" s="2"/>
@@ -14601,7 +14598,7 @@
     </row>
     <row r="106" hidden="true">
       <c r="A106" t="s" s="2">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B106" s="2"/>
       <c r="C106" t="s" s="2">
@@ -14643,7 +14640,7 @@
       </c>
       <c r="P106" s="2"/>
       <c r="Q106" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="R106" t="s" s="2">
         <v>45</v>
@@ -14720,7 +14717,7 @@
     </row>
     <row r="107" hidden="true">
       <c r="A107" t="s" s="2">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B107" s="2"/>
       <c r="C107" t="s" s="2">
@@ -14837,7 +14834,7 @@
     </row>
     <row r="108" hidden="true">
       <c r="A108" t="s" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" t="s" s="2">
@@ -14954,7 +14951,7 @@
     </row>
     <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B109" s="2"/>
       <c r="C109" t="s" s="2">
@@ -15071,7 +15068,7 @@
     </row>
     <row r="110" hidden="true">
       <c r="A110" t="s" s="2">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B110" s="2"/>
       <c r="C110" t="s" s="2">
@@ -15190,7 +15187,7 @@
     </row>
     <row r="111" hidden="true">
       <c r="A111" t="s" s="2">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B111" s="2"/>
       <c r="C111" t="s" s="2">
@@ -15309,7 +15306,7 @@
     </row>
     <row r="112" hidden="true">
       <c r="A112" t="s" s="2">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B112" s="2"/>
       <c r="C112" t="s" s="2">
@@ -15332,16 +15329,16 @@
         <v>45</v>
       </c>
       <c r="J112" t="s" s="2">
+        <v>507</v>
+      </c>
+      <c r="K112" t="s" s="2">
         <v>508</v>
       </c>
-      <c r="K112" t="s" s="2">
+      <c r="L112" t="s" s="2">
         <v>509</v>
       </c>
-      <c r="L112" t="s" s="2">
+      <c r="M112" t="s" s="2">
         <v>510</v>
-      </c>
-      <c r="M112" t="s" s="2">
-        <v>511</v>
       </c>
       <c r="N112" s="2"/>
       <c r="O112" t="s" s="2">
@@ -15391,7 +15388,7 @@
         <v>45</v>
       </c>
       <c r="AE112" t="s" s="2">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="AF112" t="s" s="2">
         <v>43</v>
@@ -15409,24 +15406,24 @@
         <v>45</v>
       </c>
       <c r="AK112" t="s" s="2">
+        <v>511</v>
+      </c>
+      <c r="AL112" t="s" s="2">
         <v>512</v>
       </c>
-      <c r="AL112" t="s" s="2">
+      <c r="AM112" t="s" s="2">
         <v>513</v>
       </c>
-      <c r="AM112" t="s" s="2">
+      <c r="AN112" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO112" t="s" s="2">
         <v>514</v>
-      </c>
-      <c r="AN112" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO112" t="s" s="2">
-        <v>515</v>
       </c>
     </row>
     <row r="113" hidden="true">
       <c r="A113" t="s" s="2">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" t="s" s="2">
@@ -15449,16 +15446,16 @@
         <v>45</v>
       </c>
       <c r="J113" t="s" s="2">
+        <v>516</v>
+      </c>
+      <c r="K113" t="s" s="2">
         <v>517</v>
       </c>
-      <c r="K113" t="s" s="2">
+      <c r="L113" t="s" s="2">
         <v>518</v>
       </c>
-      <c r="L113" t="s" s="2">
+      <c r="M113" t="s" s="2">
         <v>519</v>
-      </c>
-      <c r="M113" t="s" s="2">
-        <v>520</v>
       </c>
       <c r="N113" s="2"/>
       <c r="O113" t="s" s="2">
@@ -15508,7 +15505,7 @@
         <v>45</v>
       </c>
       <c r="AE113" t="s" s="2">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="AF113" t="s" s="2">
         <v>43</v>
@@ -15526,24 +15523,24 @@
         <v>45</v>
       </c>
       <c r="AK113" t="s" s="2">
+        <v>520</v>
+      </c>
+      <c r="AL113" t="s" s="2">
         <v>521</v>
       </c>
-      <c r="AL113" t="s" s="2">
+      <c r="AM113" t="s" s="2">
         <v>522</v>
       </c>
-      <c r="AM113" t="s" s="2">
+      <c r="AN113" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO113" t="s" s="2">
         <v>523</v>
-      </c>
-      <c r="AN113" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO113" t="s" s="2">
-        <v>524</v>
       </c>
     </row>
     <row r="114" hidden="true">
       <c r="A114" t="s" s="2">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B114" s="2"/>
       <c r="C114" t="s" s="2">
@@ -15566,19 +15563,19 @@
         <v>45</v>
       </c>
       <c r="J114" t="s" s="2">
+        <v>525</v>
+      </c>
+      <c r="K114" t="s" s="2">
         <v>526</v>
       </c>
-      <c r="K114" t="s" s="2">
+      <c r="L114" t="s" s="2">
         <v>527</v>
       </c>
-      <c r="L114" t="s" s="2">
+      <c r="M114" t="s" s="2">
         <v>528</v>
       </c>
-      <c r="M114" t="s" s="2">
+      <c r="N114" t="s" s="2">
         <v>529</v>
-      </c>
-      <c r="N114" t="s" s="2">
-        <v>530</v>
       </c>
       <c r="O114" t="s" s="2">
         <v>45</v>
@@ -15627,7 +15624,7 @@
         <v>45</v>
       </c>
       <c r="AE114" t="s" s="2">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="AF114" t="s" s="2">
         <v>43</v>
@@ -15639,19 +15636,19 @@
         <v>45</v>
       </c>
       <c r="AI114" t="s" s="2">
+        <v>530</v>
+      </c>
+      <c r="AJ114" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK114" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL114" t="s" s="2">
         <v>531</v>
       </c>
-      <c r="AJ114" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK114" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL114" t="s" s="2">
+      <c r="AM114" t="s" s="2">
         <v>532</v>
-      </c>
-      <c r="AM114" t="s" s="2">
-        <v>533</v>
       </c>
       <c r="AN114" t="s" s="2">
         <v>45</v>
@@ -15662,7 +15659,7 @@
     </row>
     <row r="115" hidden="true">
       <c r="A115" t="s" s="2">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B115" s="2"/>
       <c r="C115" t="s" s="2">
@@ -15777,7 +15774,7 @@
     </row>
     <row r="116" hidden="true">
       <c r="A116" t="s" s="2">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B116" s="2"/>
       <c r="C116" t="s" s="2">
@@ -15894,11 +15891,11 @@
     </row>
     <row r="117" hidden="true">
       <c r="A117" t="s" s="2">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B117" s="2"/>
       <c r="C117" t="s" s="2">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D117" s="2"/>
       <c r="E117" t="s" s="2">
@@ -15923,7 +15920,7 @@
         <v>108</v>
       </c>
       <c r="L117" t="s" s="2">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="M117" t="s" s="2">
         <v>105</v>
@@ -15976,7 +15973,7 @@
         <v>45</v>
       </c>
       <c r="AE117" t="s" s="2">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AF117" t="s" s="2">
         <v>43</v>
@@ -16011,7 +16008,7 @@
     </row>
     <row r="118" hidden="true">
       <c r="A118" t="s" s="2">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B118" s="2"/>
       <c r="C118" t="s" s="2">
@@ -16034,13 +16031,13 @@
         <v>45</v>
       </c>
       <c r="J118" t="s" s="2">
+        <v>540</v>
+      </c>
+      <c r="K118" t="s" s="2">
         <v>541</v>
       </c>
-      <c r="K118" t="s" s="2">
+      <c r="L118" t="s" s="2">
         <v>542</v>
-      </c>
-      <c r="L118" t="s" s="2">
-        <v>543</v>
       </c>
       <c r="M118" s="2"/>
       <c r="N118" s="2"/>
@@ -16091,7 +16088,7 @@
         <v>45</v>
       </c>
       <c r="AE118" t="s" s="2">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AF118" t="s" s="2">
         <v>43</v>
@@ -16100,22 +16097,22 @@
         <v>56</v>
       </c>
       <c r="AH118" t="s" s="2">
+        <v>543</v>
+      </c>
+      <c r="AI118" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ118" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK118" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL118" t="s" s="2">
         <v>544</v>
       </c>
-      <c r="AI118" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ118" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK118" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL118" t="s" s="2">
+      <c r="AM118" t="s" s="2">
         <v>545</v>
-      </c>
-      <c r="AM118" t="s" s="2">
-        <v>546</v>
       </c>
       <c r="AN118" t="s" s="2">
         <v>45</v>
@@ -16126,7 +16123,7 @@
     </row>
     <row r="119" hidden="true">
       <c r="A119" t="s" s="2">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B119" s="2"/>
       <c r="C119" t="s" s="2">
@@ -16149,13 +16146,13 @@
         <v>45</v>
       </c>
       <c r="J119" t="s" s="2">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="K119" t="s" s="2">
+        <v>547</v>
+      </c>
+      <c r="L119" t="s" s="2">
         <v>548</v>
-      </c>
-      <c r="L119" t="s" s="2">
-        <v>549</v>
       </c>
       <c r="M119" s="2"/>
       <c r="N119" s="2"/>
@@ -16206,7 +16203,7 @@
         <v>45</v>
       </c>
       <c r="AE119" t="s" s="2">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AF119" t="s" s="2">
         <v>43</v>
@@ -16215,22 +16212,22 @@
         <v>56</v>
       </c>
       <c r="AH119" t="s" s="2">
+        <v>543</v>
+      </c>
+      <c r="AI119" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ119" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK119" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL119" t="s" s="2">
         <v>544</v>
       </c>
-      <c r="AI119" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ119" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK119" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL119" t="s" s="2">
-        <v>545</v>
-      </c>
       <c r="AM119" t="s" s="2">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="AN119" t="s" s="2">
         <v>45</v>
@@ -16241,7 +16238,7 @@
     </row>
     <row r="120" hidden="true">
       <c r="A120" t="s" s="2">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B120" s="2"/>
       <c r="C120" t="s" s="2">
@@ -16267,16 +16264,16 @@
         <v>142</v>
       </c>
       <c r="K120" t="s" s="2">
+        <v>551</v>
+      </c>
+      <c r="L120" t="s" s="2">
         <v>552</v>
       </c>
-      <c r="L120" t="s" s="2">
+      <c r="M120" t="s" s="2">
         <v>553</v>
       </c>
-      <c r="M120" t="s" s="2">
+      <c r="N120" t="s" s="2">
         <v>554</v>
-      </c>
-      <c r="N120" t="s" s="2">
-        <v>555</v>
       </c>
       <c r="O120" t="s" s="2">
         <v>45</v>
@@ -16304,52 +16301,52 @@
         <v>79</v>
       </c>
       <c r="X120" t="s" s="2">
+        <v>555</v>
+      </c>
+      <c r="Y120" t="s" s="2">
         <v>556</v>
       </c>
-      <c r="Y120" t="s" s="2">
+      <c r="Z120" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA120" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB120" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC120" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD120" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE120" t="s" s="2">
+        <v>550</v>
+      </c>
+      <c r="AF120" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG120" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH120" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI120" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ120" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK120" t="s" s="2">
         <v>557</v>
       </c>
-      <c r="Z120" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA120" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB120" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC120" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD120" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE120" t="s" s="2">
-        <v>551</v>
-      </c>
-      <c r="AF120" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG120" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH120" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI120" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ120" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK120" t="s" s="2">
+      <c r="AL120" t="s" s="2">
         <v>558</v>
       </c>
-      <c r="AL120" t="s" s="2">
-        <v>559</v>
-      </c>
       <c r="AM120" t="s" s="2">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="AN120" t="s" s="2">
         <v>45</v>
@@ -16360,7 +16357,7 @@
     </row>
     <row r="121" hidden="true">
       <c r="A121" t="s" s="2">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B121" s="2"/>
       <c r="C121" t="s" s="2">
@@ -16386,16 +16383,16 @@
         <v>142</v>
       </c>
       <c r="K121" t="s" s="2">
+        <v>560</v>
+      </c>
+      <c r="L121" t="s" s="2">
         <v>561</v>
       </c>
-      <c r="L121" t="s" s="2">
+      <c r="M121" t="s" s="2">
         <v>562</v>
       </c>
-      <c r="M121" t="s" s="2">
+      <c r="N121" t="s" s="2">
         <v>563</v>
-      </c>
-      <c r="N121" t="s" s="2">
-        <v>564</v>
       </c>
       <c r="O121" t="s" s="2">
         <v>45</v>
@@ -16420,14 +16417,14 @@
         <v>45</v>
       </c>
       <c r="W121" t="s" s="2">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="X121" t="s" s="2">
+        <v>564</v>
+      </c>
+      <c r="Y121" t="s" s="2">
         <v>565</v>
       </c>
-      <c r="Y121" t="s" s="2">
-        <v>566</v>
-      </c>
       <c r="Z121" t="s" s="2">
         <v>45</v>
       </c>
@@ -16444,7 +16441,7 @@
         <v>45</v>
       </c>
       <c r="AE121" t="s" s="2">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="AF121" t="s" s="2">
         <v>43</v>
@@ -16462,13 +16459,13 @@
         <v>45</v>
       </c>
       <c r="AK121" t="s" s="2">
+        <v>557</v>
+      </c>
+      <c r="AL121" t="s" s="2">
         <v>558</v>
       </c>
-      <c r="AL121" t="s" s="2">
-        <v>559</v>
-      </c>
       <c r="AM121" t="s" s="2">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="AN121" t="s" s="2">
         <v>45</v>
@@ -16479,7 +16476,7 @@
     </row>
     <row r="122" hidden="true">
       <c r="A122" t="s" s="2">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B122" s="2"/>
       <c r="C122" t="s" s="2">
@@ -16502,17 +16499,17 @@
         <v>45</v>
       </c>
       <c r="J122" t="s" s="2">
+        <v>567</v>
+      </c>
+      <c r="K122" t="s" s="2">
         <v>568</v>
       </c>
-      <c r="K122" t="s" s="2">
+      <c r="L122" t="s" s="2">
         <v>569</v>
-      </c>
-      <c r="L122" t="s" s="2">
-        <v>570</v>
       </c>
       <c r="M122" s="2"/>
       <c r="N122" t="s" s="2">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="O122" t="s" s="2">
         <v>45</v>
@@ -16561,7 +16558,7 @@
         <v>45</v>
       </c>
       <c r="AE122" t="s" s="2">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="AF122" t="s" s="2">
         <v>43</v>
@@ -16585,7 +16582,7 @@
         <v>45</v>
       </c>
       <c r="AM122" t="s" s="2">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="AN122" t="s" s="2">
         <v>45</v>
@@ -16596,7 +16593,7 @@
     </row>
     <row r="123" hidden="true">
       <c r="A123" t="s" s="2">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B123" s="2"/>
       <c r="C123" t="s" s="2">
@@ -16622,10 +16619,10 @@
         <v>120</v>
       </c>
       <c r="K123" t="s" s="2">
+        <v>573</v>
+      </c>
+      <c r="L123" t="s" s="2">
         <v>574</v>
-      </c>
-      <c r="L123" t="s" s="2">
-        <v>575</v>
       </c>
       <c r="M123" s="2"/>
       <c r="N123" s="2"/>
@@ -16676,7 +16673,7 @@
         <v>45</v>
       </c>
       <c r="AE123" t="s" s="2">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="AF123" t="s" s="2">
         <v>43</v>
@@ -16697,10 +16694,10 @@
         <v>45</v>
       </c>
       <c r="AL123" t="s" s="2">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="AM123" t="s" s="2">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="AN123" t="s" s="2">
         <v>45</v>
@@ -16711,7 +16708,7 @@
     </row>
     <row r="124">
       <c r="A124" t="s" s="2">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B124" s="2"/>
       <c r="C124" t="s" s="2">
@@ -16734,19 +16731,19 @@
         <v>57</v>
       </c>
       <c r="J124" t="s" s="2">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="K124" t="s" s="2">
+        <v>577</v>
+      </c>
+      <c r="L124" t="s" s="2">
         <v>578</v>
       </c>
-      <c r="L124" t="s" s="2">
+      <c r="M124" t="s" s="2">
         <v>579</v>
       </c>
-      <c r="M124" t="s" s="2">
+      <c r="N124" t="s" s="2">
         <v>580</v>
-      </c>
-      <c r="N124" t="s" s="2">
-        <v>581</v>
       </c>
       <c r="O124" t="s" s="2">
         <v>45</v>
@@ -16795,7 +16792,7 @@
         <v>45</v>
       </c>
       <c r="AE124" t="s" s="2">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="AF124" t="s" s="2">
         <v>43</v>
@@ -16807,19 +16804,19 @@
         <v>45</v>
       </c>
       <c r="AI124" t="s" s="2">
+        <v>581</v>
+      </c>
+      <c r="AJ124" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK124" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL124" t="s" s="2">
         <v>582</v>
       </c>
-      <c r="AJ124" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK124" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL124" t="s" s="2">
+      <c r="AM124" t="s" s="2">
         <v>583</v>
-      </c>
-      <c r="AM124" t="s" s="2">
-        <v>584</v>
       </c>
       <c r="AN124" t="s" s="2">
         <v>45</v>
@@ -16830,7 +16827,7 @@
     </row>
     <row r="125" hidden="true">
       <c r="A125" t="s" s="2">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B125" s="2"/>
       <c r="C125" t="s" s="2">
@@ -16945,7 +16942,7 @@
     </row>
     <row r="126" hidden="true">
       <c r="A126" t="s" s="2">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B126" s="2"/>
       <c r="C126" t="s" s="2">
@@ -17062,11 +17059,11 @@
     </row>
     <row r="127" hidden="true">
       <c r="A127" t="s" s="2">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B127" s="2"/>
       <c r="C127" t="s" s="2">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D127" s="2"/>
       <c r="E127" t="s" s="2">
@@ -17091,7 +17088,7 @@
         <v>108</v>
       </c>
       <c r="L127" t="s" s="2">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="M127" t="s" s="2">
         <v>105</v>
@@ -17144,7 +17141,7 @@
         <v>45</v>
       </c>
       <c r="AE127" t="s" s="2">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AF127" t="s" s="2">
         <v>43</v>
@@ -17179,7 +17176,7 @@
     </row>
     <row r="128">
       <c r="A128" t="s" s="2">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B128" s="2"/>
       <c r="C128" t="s" s="2">
@@ -17205,23 +17202,23 @@
         <v>75</v>
       </c>
       <c r="K128" t="s" s="2">
+        <v>588</v>
+      </c>
+      <c r="L128" t="s" s="2">
         <v>589</v>
       </c>
-      <c r="L128" t="s" s="2">
+      <c r="M128" t="s" s="2">
         <v>590</v>
       </c>
-      <c r="M128" t="s" s="2">
+      <c r="N128" t="s" s="2">
         <v>591</v>
-      </c>
-      <c r="N128" t="s" s="2">
-        <v>592</v>
       </c>
       <c r="O128" t="s" s="2">
         <v>45</v>
       </c>
       <c r="P128" s="2"/>
       <c r="Q128" t="s" s="2">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="R128" t="s" s="2">
         <v>45</v>
@@ -17242,11 +17239,11 @@
         <v>136</v>
       </c>
       <c r="X128" t="s" s="2">
+        <v>593</v>
+      </c>
+      <c r="Y128" t="s" s="2">
         <v>594</v>
       </c>
-      <c r="Y128" t="s" s="2">
-        <v>595</v>
-      </c>
       <c r="Z128" t="s" s="2">
         <v>45</v>
       </c>
@@ -17263,7 +17260,7 @@
         <v>45</v>
       </c>
       <c r="AE128" t="s" s="2">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="AF128" t="s" s="2">
         <v>43</v>
@@ -17287,7 +17284,7 @@
         <v>99</v>
       </c>
       <c r="AM128" t="s" s="2">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="AN128" t="s" s="2">
         <v>45</v>
@@ -17298,7 +17295,7 @@
     </row>
     <row r="129">
       <c r="A129" t="s" s="2">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B129" s="2"/>
       <c r="C129" t="s" s="2">
@@ -17321,13 +17318,13 @@
         <v>45</v>
       </c>
       <c r="J129" t="s" s="2">
+        <v>597</v>
+      </c>
+      <c r="K129" t="s" s="2">
         <v>598</v>
       </c>
-      <c r="K129" t="s" s="2">
+      <c r="L129" t="s" s="2">
         <v>599</v>
-      </c>
-      <c r="L129" t="s" s="2">
-        <v>600</v>
       </c>
       <c r="M129" s="2"/>
       <c r="N129" s="2"/>
@@ -17378,7 +17375,7 @@
         <v>45</v>
       </c>
       <c r="AE129" t="s" s="2">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="AF129" t="s" s="2">
         <v>56</v>
@@ -17402,7 +17399,7 @@
         <v>45</v>
       </c>
       <c r="AM129" t="s" s="2">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="AN129" t="s" s="2">
         <v>45</v>
@@ -17413,7 +17410,7 @@
     </row>
     <row r="130">
       <c r="A130" t="s" s="2">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B130" s="2"/>
       <c r="C130" t="s" s="2">
@@ -17436,19 +17433,19 @@
         <v>57</v>
       </c>
       <c r="J130" t="s" s="2">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="K130" t="s" s="2">
+        <v>602</v>
+      </c>
+      <c r="L130" t="s" s="2">
         <v>603</v>
       </c>
-      <c r="L130" t="s" s="2">
+      <c r="M130" t="s" s="2">
         <v>604</v>
       </c>
-      <c r="M130" t="s" s="2">
+      <c r="N130" t="s" s="2">
         <v>605</v>
-      </c>
-      <c r="N130" t="s" s="2">
-        <v>606</v>
       </c>
       <c r="O130" t="s" s="2">
         <v>45</v>
@@ -17497,7 +17494,7 @@
         <v>45</v>
       </c>
       <c r="AE130" t="s" s="2">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="AF130" t="s" s="2">
         <v>43</v>
@@ -17509,7 +17506,7 @@
         <v>45</v>
       </c>
       <c r="AI130" t="s" s="2">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AJ130" t="s" s="2">
         <v>45</v>
@@ -17518,10 +17515,10 @@
         <v>45</v>
       </c>
       <c r="AL130" t="s" s="2">
+        <v>606</v>
+      </c>
+      <c r="AM130" t="s" s="2">
         <v>607</v>
-      </c>
-      <c r="AM130" t="s" s="2">
-        <v>608</v>
       </c>
       <c r="AN130" t="s" s="2">
         <v>45</v>
@@ -17532,7 +17529,7 @@
     </row>
     <row r="131" hidden="true">
       <c r="A131" t="s" s="2">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B131" s="2"/>
       <c r="C131" t="s" s="2">
@@ -17647,7 +17644,7 @@
     </row>
     <row r="132" hidden="true">
       <c r="A132" t="s" s="2">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B132" s="2"/>
       <c r="C132" t="s" s="2">
@@ -17764,11 +17761,11 @@
     </row>
     <row r="133" hidden="true">
       <c r="A133" t="s" s="2">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B133" s="2"/>
       <c r="C133" t="s" s="2">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D133" s="2"/>
       <c r="E133" t="s" s="2">
@@ -17793,7 +17790,7 @@
         <v>108</v>
       </c>
       <c r="L133" t="s" s="2">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="M133" t="s" s="2">
         <v>105</v>
@@ -17846,7 +17843,7 @@
         <v>45</v>
       </c>
       <c r="AE133" t="s" s="2">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AF133" t="s" s="2">
         <v>43</v>
@@ -17881,7 +17878,7 @@
     </row>
     <row r="134">
       <c r="A134" t="s" s="2">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B134" s="2"/>
       <c r="C134" t="s" s="2">
@@ -17907,10 +17904,10 @@
         <v>142</v>
       </c>
       <c r="K134" t="s" s="2">
+        <v>612</v>
+      </c>
+      <c r="L134" t="s" s="2">
         <v>613</v>
-      </c>
-      <c r="L134" t="s" s="2">
-        <v>614</v>
       </c>
       <c r="M134" s="2"/>
       <c r="N134" t="s" s="2">
@@ -17942,7 +17939,7 @@
         <v>79</v>
       </c>
       <c r="X134" t="s" s="2">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="Y134" t="s" s="2">
         <v>279</v>
@@ -17963,7 +17960,7 @@
         <v>45</v>
       </c>
       <c r="AE134" t="s" s="2">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="AF134" t="s" s="2">
         <v>56</v>
@@ -17981,7 +17978,7 @@
         <v>45</v>
       </c>
       <c r="AK134" t="s" s="2">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AL134" t="s" s="2">
         <v>282</v>
@@ -17998,7 +17995,7 @@
     </row>
     <row r="135" hidden="true">
       <c r="A135" t="s" s="2">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B135" s="2"/>
       <c r="C135" t="s" s="2">
@@ -18113,7 +18110,7 @@
     </row>
     <row r="136" hidden="true">
       <c r="A136" t="s" s="2">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B136" s="2"/>
       <c r="C136" t="s" s="2">
@@ -18230,7 +18227,7 @@
     </row>
     <row r="137" hidden="true">
       <c r="A137" t="s" s="2">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B137" s="2"/>
       <c r="C137" t="s" s="2">
@@ -18347,7 +18344,7 @@
     </row>
     <row r="138" hidden="true">
       <c r="A138" t="s" s="2">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B138" t="s" s="2">
         <v>290</v>
@@ -18412,7 +18409,7 @@
         <v>79</v>
       </c>
       <c r="X138" t="s" s="2">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="Y138" t="s" s="2">
         <v>279</v>
@@ -18468,7 +18465,7 @@
     </row>
     <row r="139" hidden="true">
       <c r="A139" t="s" s="2">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B139" s="2"/>
       <c r="C139" t="s" s="2">
@@ -18583,7 +18580,7 @@
     </row>
     <row r="140" hidden="true">
       <c r="A140" t="s" s="2">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B140" s="2"/>
       <c r="C140" t="s" s="2">
@@ -18700,7 +18697,7 @@
     </row>
     <row r="141" hidden="true">
       <c r="A141" t="s" s="2">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B141" s="2"/>
       <c r="C141" t="s" s="2">
@@ -18742,7 +18739,7 @@
       </c>
       <c r="P141" s="2"/>
       <c r="Q141" t="s" s="2">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="R141" t="s" s="2">
         <v>45</v>
@@ -18819,7 +18816,7 @@
     </row>
     <row r="142" hidden="true">
       <c r="A142" t="s" s="2">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B142" s="2"/>
       <c r="C142" t="s" s="2">
@@ -18936,7 +18933,7 @@
     </row>
     <row r="143" hidden="true">
       <c r="A143" t="s" s="2">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B143" s="2"/>
       <c r="C143" t="s" s="2">
@@ -19053,7 +19050,7 @@
     </row>
     <row r="144" hidden="true">
       <c r="A144" t="s" s="2">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B144" s="2"/>
       <c r="C144" t="s" s="2">
@@ -19170,7 +19167,7 @@
     </row>
     <row r="145" hidden="true">
       <c r="A145" t="s" s="2">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B145" s="2"/>
       <c r="C145" t="s" s="2">
@@ -19289,10 +19286,10 @@
     </row>
     <row r="146" hidden="true">
       <c r="A146" t="s" s="2">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B146" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C146" t="s" s="2">
         <v>45</v>
@@ -19410,7 +19407,7 @@
     </row>
     <row r="147" hidden="true">
       <c r="A147" t="s" s="2">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B147" s="2"/>
       <c r="C147" t="s" s="2">
@@ -19525,7 +19522,7 @@
     </row>
     <row r="148" hidden="true">
       <c r="A148" t="s" s="2">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B148" s="2"/>
       <c r="C148" t="s" s="2">
@@ -19551,10 +19548,10 @@
         <v>102</v>
       </c>
       <c r="K148" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="L148" t="s" s="2">
         <v>302</v>
-      </c>
-      <c r="L148" t="s" s="2">
-        <v>303</v>
       </c>
       <c r="M148" s="2"/>
       <c r="N148" s="2"/>
@@ -19640,10 +19637,10 @@
     </row>
     <row r="149" hidden="true">
       <c r="A149" t="s" s="2">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B149" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C149" t="s" s="2">
         <v>45</v>
@@ -19665,13 +19662,13 @@
         <v>45</v>
       </c>
       <c r="J149" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="K149" t="s" s="2">
         <v>305</v>
       </c>
-      <c r="K149" t="s" s="2">
+      <c r="L149" t="s" s="2">
         <v>306</v>
-      </c>
-      <c r="L149" t="s" s="2">
-        <v>307</v>
       </c>
       <c r="M149" s="2"/>
       <c r="N149" s="2"/>
@@ -19757,7 +19754,7 @@
     </row>
     <row r="150" hidden="true">
       <c r="A150" t="s" s="2">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B150" s="2"/>
       <c r="C150" t="s" s="2">
@@ -19799,7 +19796,7 @@
       </c>
       <c r="P150" s="2"/>
       <c r="Q150" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="R150" t="s" s="2">
         <v>45</v>
@@ -19876,7 +19873,7 @@
     </row>
     <row r="151" hidden="true">
       <c r="A151" t="s" s="2">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B151" s="2"/>
       <c r="C151" t="s" s="2">
@@ -19993,7 +19990,7 @@
     </row>
     <row r="152" hidden="true">
       <c r="A152" t="s" s="2">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B152" s="2"/>
       <c r="C152" t="s" s="2">
@@ -20110,7 +20107,7 @@
     </row>
     <row r="153" hidden="true">
       <c r="A153" t="s" s="2">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B153" s="2"/>
       <c r="C153" t="s" s="2">
@@ -20227,7 +20224,7 @@
     </row>
     <row r="154" hidden="true">
       <c r="A154" t="s" s="2">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B154" s="2"/>
       <c r="C154" t="s" s="2">
@@ -20346,7 +20343,7 @@
     </row>
     <row r="155" hidden="true">
       <c r="A155" t="s" s="2">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B155" s="2"/>
       <c r="C155" t="s" s="2">
@@ -20465,7 +20462,7 @@
     </row>
     <row r="156" hidden="true">
       <c r="A156" t="s" s="2">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B156" s="2"/>
       <c r="C156" t="s" s="2">
@@ -20488,19 +20485,19 @@
         <v>57</v>
       </c>
       <c r="J156" t="s" s="2">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="K156" t="s" s="2">
+        <v>628</v>
+      </c>
+      <c r="L156" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="M156" t="s" s="2">
         <v>629</v>
       </c>
-      <c r="L156" t="s" s="2">
-        <v>364</v>
-      </c>
-      <c r="M156" t="s" s="2">
-        <v>630</v>
-      </c>
       <c r="N156" t="s" s="2">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="O156" t="s" s="2">
         <v>45</v>
@@ -20537,17 +20534,17 @@
         <v>45</v>
       </c>
       <c r="AA156" t="s" s="2">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AB156" s="2"/>
       <c r="AC156" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD156" t="s" s="2">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AE156" t="s" s="2">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="AF156" t="s" s="2">
         <v>43</v>
@@ -20565,27 +20562,27 @@
         <v>45</v>
       </c>
       <c r="AK156" t="s" s="2">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="AL156" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="AM156" t="s" s="2">
         <v>372</v>
       </c>
-      <c r="AM156" t="s" s="2">
+      <c r="AN156" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO156" t="s" s="2">
         <v>373</v>
-      </c>
-      <c r="AN156" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO156" t="s" s="2">
-        <v>374</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="s" s="2">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B157" t="s" s="2">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C157" t="s" s="2">
         <v>45</v>
@@ -20607,19 +20604,19 @@
         <v>57</v>
       </c>
       <c r="J157" t="s" s="2">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="K157" t="s" s="2">
+        <v>628</v>
+      </c>
+      <c r="L157" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="M157" t="s" s="2">
         <v>629</v>
       </c>
-      <c r="L157" t="s" s="2">
-        <v>364</v>
-      </c>
-      <c r="M157" t="s" s="2">
-        <v>630</v>
-      </c>
       <c r="N157" t="s" s="2">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="O157" t="s" s="2">
         <v>45</v>
@@ -20647,11 +20644,11 @@
         <v>136</v>
       </c>
       <c r="X157" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="Y157" t="s" s="2">
         <v>376</v>
       </c>
-      <c r="Y157" t="s" s="2">
-        <v>377</v>
-      </c>
       <c r="Z157" t="s" s="2">
         <v>45</v>
       </c>
@@ -20668,7 +20665,7 @@
         <v>45</v>
       </c>
       <c r="AE157" t="s" s="2">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="AF157" t="s" s="2">
         <v>43</v>
@@ -20686,24 +20683,24 @@
         <v>45</v>
       </c>
       <c r="AK157" t="s" s="2">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="AL157" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="AM157" t="s" s="2">
         <v>372</v>
       </c>
-      <c r="AM157" t="s" s="2">
+      <c r="AN157" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO157" t="s" s="2">
         <v>373</v>
-      </c>
-      <c r="AN157" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO157" t="s" s="2">
-        <v>374</v>
       </c>
     </row>
     <row r="158" hidden="true">
       <c r="A158" t="s" s="2">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B158" s="2"/>
       <c r="C158" t="s" s="2">
@@ -20818,7 +20815,7 @@
     </row>
     <row r="159" hidden="true">
       <c r="A159" t="s" s="2">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B159" s="2"/>
       <c r="C159" t="s" s="2">
@@ -20935,7 +20932,7 @@
     </row>
     <row r="160">
       <c r="A160" t="s" s="2">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B160" s="2"/>
       <c r="C160" t="s" s="2">
@@ -20958,19 +20955,19 @@
         <v>57</v>
       </c>
       <c r="J160" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="K160" t="s" s="2">
         <v>381</v>
       </c>
-      <c r="K160" t="s" s="2">
+      <c r="L160" t="s" s="2">
         <v>382</v>
       </c>
-      <c r="L160" t="s" s="2">
+      <c r="M160" t="s" s="2">
         <v>383</v>
       </c>
-      <c r="M160" t="s" s="2">
+      <c r="N160" t="s" s="2">
         <v>384</v>
-      </c>
-      <c r="N160" t="s" s="2">
-        <v>385</v>
       </c>
       <c r="O160" t="s" s="2">
         <v>45</v>
@@ -21019,31 +21016,31 @@
         <v>45</v>
       </c>
       <c r="AE160" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="AF160" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG160" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH160" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI160" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ160" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK160" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL160" t="s" s="2">
         <v>386</v>
       </c>
-      <c r="AF160" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG160" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH160" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI160" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ160" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK160" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL160" t="s" s="2">
+      <c r="AM160" t="s" s="2">
         <v>387</v>
-      </c>
-      <c r="AM160" t="s" s="2">
-        <v>388</v>
       </c>
       <c r="AN160" t="s" s="2">
         <v>45</v>
@@ -21054,7 +21051,7 @@
     </row>
     <row r="161" hidden="true">
       <c r="A161" t="s" s="2">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B161" s="2"/>
       <c r="C161" t="s" s="2">
@@ -21080,22 +21077,22 @@
         <v>75</v>
       </c>
       <c r="K161" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="L161" t="s" s="2">
         <v>390</v>
       </c>
-      <c r="L161" t="s" s="2">
+      <c r="M161" t="s" s="2">
         <v>391</v>
       </c>
-      <c r="M161" t="s" s="2">
+      <c r="N161" t="s" s="2">
         <v>392</v>
       </c>
-      <c r="N161" t="s" s="2">
+      <c r="O161" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P161" t="s" s="2">
         <v>393</v>
-      </c>
-      <c r="O161" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="P161" t="s" s="2">
-        <v>394</v>
       </c>
       <c r="Q161" t="s" s="2">
         <v>45</v>
@@ -21119,52 +21116,52 @@
         <v>136</v>
       </c>
       <c r="X161" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="Y161" t="s" s="2">
         <v>395</v>
       </c>
-      <c r="Y161" t="s" s="2">
+      <c r="Z161" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA161" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB161" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC161" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD161" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE161" t="s" s="2">
         <v>396</v>
       </c>
-      <c r="Z161" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA161" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB161" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC161" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD161" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE161" t="s" s="2">
+      <c r="AF161" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG161" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH161" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI161" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ161" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK161" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL161" t="s" s="2">
         <v>397</v>
       </c>
-      <c r="AF161" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG161" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH161" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI161" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ161" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK161" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL161" t="s" s="2">
+      <c r="AM161" t="s" s="2">
         <v>398</v>
-      </c>
-      <c r="AM161" t="s" s="2">
-        <v>399</v>
       </c>
       <c r="AN161" t="s" s="2">
         <v>45</v>
@@ -21175,7 +21172,7 @@
     </row>
     <row r="162">
       <c r="A162" t="s" s="2">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B162" s="2"/>
       <c r="C162" t="s" s="2">
@@ -21201,14 +21198,14 @@
         <v>120</v>
       </c>
       <c r="K162" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="L162" t="s" s="2">
         <v>401</v>
-      </c>
-      <c r="L162" t="s" s="2">
-        <v>402</v>
       </c>
       <c r="M162" s="2"/>
       <c r="N162" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="O162" t="s" s="2">
         <v>45</v>
@@ -21257,31 +21254,31 @@
         <v>45</v>
       </c>
       <c r="AE162" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="AF162" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG162" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH162" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI162" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ162" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK162" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL162" t="s" s="2">
         <v>404</v>
       </c>
-      <c r="AF162" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG162" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH162" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI162" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ162" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK162" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL162" t="s" s="2">
+      <c r="AM162" t="s" s="2">
         <v>405</v>
-      </c>
-      <c r="AM162" t="s" s="2">
-        <v>406</v>
       </c>
       <c r="AN162" t="s" s="2">
         <v>45</v>
@@ -21292,7 +21289,7 @@
     </row>
     <row r="163">
       <c r="A163" t="s" s="2">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B163" s="2"/>
       <c r="C163" t="s" s="2">
@@ -21318,87 +21315,87 @@
         <v>69</v>
       </c>
       <c r="K163" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="L163" t="s" s="2">
         <v>408</v>
-      </c>
-      <c r="L163" t="s" s="2">
-        <v>409</v>
       </c>
       <c r="M163" s="2"/>
       <c r="N163" t="s" s="2">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="O163" t="s" s="2">
         <v>45</v>
       </c>
       <c r="P163" s="2"/>
       <c r="Q163" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="R163" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S163" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T163" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U163" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V163" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W163" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X163" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y163" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z163" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA163" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB163" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC163" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD163" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE163" t="s" s="2">
         <v>411</v>
       </c>
-      <c r="R163" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="S163" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T163" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U163" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V163" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W163" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X163" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Y163" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Z163" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA163" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB163" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC163" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD163" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE163" t="s" s="2">
+      <c r="AF163" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG163" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH163" t="s" s="2">
         <v>412</v>
       </c>
-      <c r="AF163" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG163" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH163" t="s" s="2">
+      <c r="AI163" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ163" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK163" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL163" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="AM163" t="s" s="2">
         <v>413</v>
-      </c>
-      <c r="AI163" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ163" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK163" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL163" t="s" s="2">
-        <v>405</v>
-      </c>
-      <c r="AM163" t="s" s="2">
-        <v>414</v>
       </c>
       <c r="AN163" t="s" s="2">
         <v>45</v>
@@ -21409,7 +21406,7 @@
     </row>
     <row r="164">
       <c r="A164" t="s" s="2">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B164" s="2"/>
       <c r="C164" t="s" s="2">
@@ -21435,16 +21432,16 @@
         <v>75</v>
       </c>
       <c r="K164" t="s" s="2">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="L164" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="M164" t="s" s="2">
         <v>417</v>
       </c>
-      <c r="M164" t="s" s="2">
+      <c r="N164" t="s" s="2">
         <v>418</v>
-      </c>
-      <c r="N164" t="s" s="2">
-        <v>419</v>
       </c>
       <c r="O164" t="s" s="2">
         <v>45</v>
@@ -21472,11 +21469,11 @@
         <v>136</v>
       </c>
       <c r="X164" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="Y164" t="s" s="2">
         <v>376</v>
       </c>
-      <c r="Y164" t="s" s="2">
-        <v>377</v>
-      </c>
       <c r="Z164" t="s" s="2">
         <v>45</v>
       </c>
@@ -21493,31 +21490,31 @@
         <v>45</v>
       </c>
       <c r="AE164" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="AF164" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG164" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH164" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI164" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ164" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK164" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL164" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="AM164" t="s" s="2">
         <v>421</v>
-      </c>
-      <c r="AF164" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG164" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH164" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI164" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ164" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK164" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL164" t="s" s="2">
-        <v>405</v>
-      </c>
-      <c r="AM164" t="s" s="2">
-        <v>422</v>
       </c>
       <c r="AN164" t="s" s="2">
         <v>45</v>
@@ -21528,7 +21525,7 @@
     </row>
     <row r="165">
       <c r="A165" t="s" s="2">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B165" s="2"/>
       <c r="C165" t="s" s="2">
@@ -21554,16 +21551,16 @@
         <v>142</v>
       </c>
       <c r="K165" t="s" s="2">
+        <v>640</v>
+      </c>
+      <c r="L165" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="M165" t="s" s="2">
         <v>641</v>
       </c>
-      <c r="L165" t="s" s="2">
-        <v>425</v>
-      </c>
-      <c r="M165" t="s" s="2">
-        <v>642</v>
-      </c>
       <c r="N165" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="O165" t="s" s="2">
         <v>45</v>
@@ -21591,11 +21588,11 @@
         <v>79</v>
       </c>
       <c r="X165" t="s" s="2">
+        <v>642</v>
+      </c>
+      <c r="Y165" t="s" s="2">
         <v>643</v>
       </c>
-      <c r="Y165" t="s" s="2">
-        <v>644</v>
-      </c>
       <c r="Z165" t="s" s="2">
         <v>45</v>
       </c>
@@ -21612,7 +21609,7 @@
         <v>45</v>
       </c>
       <c r="AE165" t="s" s="2">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="AF165" t="s" s="2">
         <v>43</v>
@@ -21621,7 +21618,7 @@
         <v>56</v>
       </c>
       <c r="AH165" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AI165" t="s" s="2">
         <v>45</v>
@@ -21636,7 +21633,7 @@
         <v>99</v>
       </c>
       <c r="AM165" t="s" s="2">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="AN165" t="s" s="2">
         <v>45</v>
@@ -21647,7 +21644,7 @@
     </row>
     <row r="166" hidden="true">
       <c r="A166" t="s" s="2">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B166" s="2"/>
       <c r="C166" t="s" s="2">
@@ -21762,7 +21759,7 @@
     </row>
     <row r="167" hidden="true">
       <c r="A167" t="s" s="2">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B167" s="2"/>
       <c r="C167" t="s" s="2">
@@ -21879,7 +21876,7 @@
     </row>
     <row r="168" hidden="true">
       <c r="A168" t="s" s="2">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B168" s="2"/>
       <c r="C168" t="s" s="2">
@@ -21998,7 +21995,7 @@
     </row>
     <row r="169" hidden="true">
       <c r="A169" t="s" s="2">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B169" s="2"/>
       <c r="C169" t="s" s="2">
@@ -22113,7 +22110,7 @@
     </row>
     <row r="170" hidden="true">
       <c r="A170" t="s" s="2">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B170" s="2"/>
       <c r="C170" t="s" s="2">
@@ -22230,7 +22227,7 @@
     </row>
     <row r="171" hidden="true">
       <c r="A171" t="s" s="2">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B171" s="2"/>
       <c r="C171" t="s" s="2">
@@ -22349,7 +22346,7 @@
     </row>
     <row r="172" hidden="true">
       <c r="A172" t="s" s="2">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B172" s="2"/>
       <c r="C172" t="s" s="2">
@@ -22466,7 +22463,7 @@
     </row>
     <row r="173" hidden="true">
       <c r="A173" t="s" s="2">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B173" s="2"/>
       <c r="C173" t="s" s="2">
@@ -22583,7 +22580,7 @@
     </row>
     <row r="174" hidden="true">
       <c r="A174" t="s" s="2">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B174" s="2"/>
       <c r="C174" t="s" s="2">
@@ -22700,7 +22697,7 @@
     </row>
     <row r="175" hidden="true">
       <c r="A175" t="s" s="2">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B175" s="2"/>
       <c r="C175" t="s" s="2">
@@ -22819,7 +22816,7 @@
     </row>
     <row r="176" hidden="true">
       <c r="A176" t="s" s="2">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B176" s="2"/>
       <c r="C176" t="s" s="2">
@@ -22938,11 +22935,11 @@
     </row>
     <row r="177" hidden="true">
       <c r="A177" t="s" s="2">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B177" s="2"/>
       <c r="C177" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D177" s="2"/>
       <c r="E177" t="s" s="2">
@@ -22964,16 +22961,16 @@
         <v>142</v>
       </c>
       <c r="K177" t="s" s="2">
+        <v>443</v>
+      </c>
+      <c r="L177" t="s" s="2">
         <v>444</v>
       </c>
-      <c r="L177" t="s" s="2">
+      <c r="M177" t="s" s="2">
+        <v>656</v>
+      </c>
+      <c r="N177" t="s" s="2">
         <v>445</v>
-      </c>
-      <c r="M177" t="s" s="2">
-        <v>657</v>
-      </c>
-      <c r="N177" t="s" s="2">
-        <v>446</v>
       </c>
       <c r="O177" t="s" s="2">
         <v>45</v>
@@ -23001,11 +22998,11 @@
         <v>79</v>
       </c>
       <c r="X177" t="s" s="2">
+        <v>657</v>
+      </c>
+      <c r="Y177" t="s" s="2">
         <v>658</v>
       </c>
-      <c r="Y177" t="s" s="2">
-        <v>659</v>
-      </c>
       <c r="Z177" t="s" s="2">
         <v>45</v>
       </c>
@@ -23022,7 +23019,7 @@
         <v>45</v>
       </c>
       <c r="AE177" t="s" s="2">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="AF177" t="s" s="2">
         <v>43</v>
@@ -23040,24 +23037,24 @@
         <v>45</v>
       </c>
       <c r="AK177" t="s" s="2">
+        <v>447</v>
+      </c>
+      <c r="AL177" t="s" s="2">
         <v>448</v>
       </c>
-      <c r="AL177" t="s" s="2">
+      <c r="AM177" t="s" s="2">
         <v>449</v>
       </c>
-      <c r="AM177" t="s" s="2">
+      <c r="AN177" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO177" t="s" s="2">
         <v>450</v>
-      </c>
-      <c r="AN177" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO177" t="s" s="2">
-        <v>451</v>
       </c>
     </row>
     <row r="178" hidden="true">
       <c r="A178" t="s" s="2">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B178" s="2"/>
       <c r="C178" t="s" s="2">
@@ -23083,16 +23080,16 @@
         <v>45</v>
       </c>
       <c r="K178" t="s" s="2">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="L178" t="s" s="2">
+        <v>527</v>
+      </c>
+      <c r="M178" t="s" s="2">
         <v>528</v>
       </c>
-      <c r="M178" t="s" s="2">
+      <c r="N178" t="s" s="2">
         <v>529</v>
-      </c>
-      <c r="N178" t="s" s="2">
-        <v>530</v>
       </c>
       <c r="O178" t="s" s="2">
         <v>45</v>
@@ -23141,7 +23138,7 @@
         <v>45</v>
       </c>
       <c r="AE178" t="s" s="2">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="AF178" t="s" s="2">
         <v>43</v>
@@ -23162,10 +23159,10 @@
         <v>45</v>
       </c>
       <c r="AL178" t="s" s="2">
+        <v>531</v>
+      </c>
+      <c r="AM178" t="s" s="2">
         <v>532</v>
-      </c>
-      <c r="AM178" t="s" s="2">
-        <v>533</v>
       </c>
       <c r="AN178" t="s" s="2">
         <v>45</v>

</xml_diff>